<commit_message>
updated repository/ add new tabs to the data
</commit_message>
<xml_diff>
--- a/data/Florida-International-U.xlsx
+++ b/data/Florida-International-U.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://olddominion-my.sharepoint.com/personal/bllin001_odu_edu/Documents/VMASC/Projects/nsf-univerisitites/grad-postdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{D155F73D-045F-1147-B375-9AD929F188BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66B7FB70-0A96-F64A-9763-9EB3400ED6B6}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{D155F73D-045F-1147-B375-9AD929F188BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9576BB5B-F3C2-3B49-A6B3-AD346931E986}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="2720" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{028BD6CC-7404-114A-9DEB-BB23B3B9A9CD}"/>
+    <workbookView xWindow="-30100" yWindow="2880" windowWidth="29940" windowHeight="18580" activeTab="1" xr2:uid="{028BD6CC-7404-114A-9DEB-BB23B3B9A9CD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Graduate Students" sheetId="1" r:id="rId1"/>
-    <sheet name="Source" sheetId="2" r:id="rId2"/>
-    <sheet name="Postdoctorates" sheetId="4" r:id="rId3"/>
+    <sheet name="Earned Doctorates" sheetId="5" r:id="rId1"/>
+    <sheet name="Full-time Graduate Students" sheetId="1" r:id="rId2"/>
+    <sheet name="Part-time Graduate Students" sheetId="6" r:id="rId3"/>
+    <sheet name="Source" sheetId="2" r:id="rId4"/>
+    <sheet name="Postdoctorates" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="147">
   <si>
     <t>All races</t>
   </si>
@@ -194,13 +196,298 @@
   </si>
   <si>
     <t>Personal resources</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>All fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Science and engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Life science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Agricultural sciences</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Biological sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Health sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Physical sciences and earth sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Chemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Earth, atmospheric, and ocean sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Physics and astronomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Mathematics and computer sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Computer sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Mathematics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Psychology and social sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Psychology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Anthropology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Economics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Political science and government</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Sociology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Other social sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Biological/biomedical sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Chemical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Civil engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Electrical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Materials/metallurgical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Mechanical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Other engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Non-science and engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Education research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Teacher education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Teaching fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Other education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Humanities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Foreign languages &amp; literature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Other humanities and arts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Business management/administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Fields not elsewhere classified (nec)</t>
+  </si>
+  <si>
+    <t>All part-time students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  U.S. citizens and permanent residents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Hispanic or Latino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Not Hispanic or Latino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      American Indian or Alaska Native</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Asian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Black or African American</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Native Hawaiian or Other Pacific Islander</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      More than one race</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Unknown ethnicity and race</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Temporary visa holders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Science and engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Agricultural and veterinary sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Biological and biomedical sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Computer and information sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Family and consumer sciences and human sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Geosciences, atmospheric sciences, and ocean sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Mathematics and statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Multidisciplinary and interdisciplinary studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Natural resources and conservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Psychology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Physical sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Social sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Aerospace, aeronautical, and astronautical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Biological, biomedical, and biosystems engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Chemical, petroleum, and chemical-related engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Civil, environmental, transportation and related engineering fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Electrical, electronics, communications and computer engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Industrial, manufacturing, systems engineering and operations research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Mechanical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Metallurgical, mining, materials and related engineering fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Other engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Clinical medicine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Other health</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,16 +510,27 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -255,16 +553,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,11 +935,1531 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794EA216-2266-5D46-BE14-54B114AF50D5}">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="7">
+        <v>208</v>
+      </c>
+      <c r="C2" s="7">
+        <v>193</v>
+      </c>
+      <c r="D2" s="7">
+        <v>186</v>
+      </c>
+      <c r="E2" s="7">
+        <v>204</v>
+      </c>
+      <c r="F2" s="7">
+        <v>187</v>
+      </c>
+      <c r="G2" s="7">
+        <v>184</v>
+      </c>
+      <c r="H2" s="7">
+        <v>138</v>
+      </c>
+      <c r="I2" s="7">
+        <v>173</v>
+      </c>
+      <c r="J2" s="7">
+        <v>143</v>
+      </c>
+      <c r="K2" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="7">
+        <v>172</v>
+      </c>
+      <c r="C3" s="7">
+        <v>149</v>
+      </c>
+      <c r="D3" s="7">
+        <v>145</v>
+      </c>
+      <c r="E3" s="7">
+        <v>159</v>
+      </c>
+      <c r="F3" s="7">
+        <v>157</v>
+      </c>
+      <c r="G3" s="7">
+        <v>153</v>
+      </c>
+      <c r="H3" s="7">
+        <v>115</v>
+      </c>
+      <c r="I3" s="7">
+        <v>141</v>
+      </c>
+      <c r="J3" s="7">
+        <v>123</v>
+      </c>
+      <c r="K3" s="7">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="7">
+        <v>130</v>
+      </c>
+      <c r="C4" s="7">
+        <v>112</v>
+      </c>
+      <c r="D4" s="7">
+        <v>102</v>
+      </c>
+      <c r="E4" s="7">
+        <v>126</v>
+      </c>
+      <c r="F4" s="7">
+        <v>116</v>
+      </c>
+      <c r="G4" s="7">
+        <v>111</v>
+      </c>
+      <c r="H4" s="7">
+        <v>79</v>
+      </c>
+      <c r="I4" s="7">
+        <v>112</v>
+      </c>
+      <c r="J4" s="7">
+        <v>94</v>
+      </c>
+      <c r="K4" s="7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="7">
+        <v>39</v>
+      </c>
+      <c r="C5" s="7">
+        <v>32</v>
+      </c>
+      <c r="D5" s="7">
+        <v>33</v>
+      </c>
+      <c r="E5" s="7">
+        <v>46</v>
+      </c>
+      <c r="F5" s="7">
+        <v>45</v>
+      </c>
+      <c r="G5" s="7">
+        <v>40</v>
+      </c>
+      <c r="H5" s="7">
+        <v>23</v>
+      </c>
+      <c r="I5" s="7">
+        <v>37</v>
+      </c>
+      <c r="J5" s="7">
+        <v>23</v>
+      </c>
+      <c r="K5" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="7">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="7">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7">
+        <v>21</v>
+      </c>
+      <c r="D7" s="7">
+        <v>25</v>
+      </c>
+      <c r="E7" s="7">
+        <v>31</v>
+      </c>
+      <c r="F7" s="7">
+        <v>31</v>
+      </c>
+      <c r="G7" s="7">
+        <v>26</v>
+      </c>
+      <c r="H7" s="7">
+        <v>18</v>
+      </c>
+      <c r="I7" s="7">
+        <v>22</v>
+      </c>
+      <c r="J7" s="7">
+        <v>17</v>
+      </c>
+      <c r="K7" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="7">
+        <v>13</v>
+      </c>
+      <c r="C8" s="7">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7">
+        <v>6</v>
+      </c>
+      <c r="E8" s="7">
+        <v>14</v>
+      </c>
+      <c r="F8" s="7">
+        <v>13</v>
+      </c>
+      <c r="G8" s="7">
+        <v>13</v>
+      </c>
+      <c r="H8" s="7">
+        <v>5</v>
+      </c>
+      <c r="I8" s="7">
+        <v>13</v>
+      </c>
+      <c r="J8" s="7">
+        <v>6</v>
+      </c>
+      <c r="K8" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="7">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7">
+        <v>22</v>
+      </c>
+      <c r="D9" s="7">
+        <v>20</v>
+      </c>
+      <c r="E9" s="7">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7">
+        <v>28</v>
+      </c>
+      <c r="G9" s="7">
+        <v>20</v>
+      </c>
+      <c r="H9" s="7">
+        <v>23</v>
+      </c>
+      <c r="I9" s="7">
+        <v>21</v>
+      </c>
+      <c r="J9" s="7">
+        <v>32</v>
+      </c>
+      <c r="K9" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="7">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7">
+        <v>12</v>
+      </c>
+      <c r="E10" s="7">
+        <v>20</v>
+      </c>
+      <c r="F10" s="7">
+        <v>20</v>
+      </c>
+      <c r="G10" s="7">
+        <v>12</v>
+      </c>
+      <c r="H10" s="7">
+        <v>13</v>
+      </c>
+      <c r="I10" s="7">
+        <v>12</v>
+      </c>
+      <c r="J10" s="7">
+        <v>17</v>
+      </c>
+      <c r="K10" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7">
+        <v>6</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7">
+        <v>7</v>
+      </c>
+      <c r="F11" s="7">
+        <v>4</v>
+      </c>
+      <c r="G11" s="7">
+        <v>3</v>
+      </c>
+      <c r="H11" s="7">
+        <v>6</v>
+      </c>
+      <c r="I11" s="7">
+        <v>5</v>
+      </c>
+      <c r="J11" s="7">
+        <v>8</v>
+      </c>
+      <c r="K11" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="7">
+        <v>5</v>
+      </c>
+      <c r="C12" s="7">
+        <v>8</v>
+      </c>
+      <c r="D12" s="7">
+        <v>3</v>
+      </c>
+      <c r="E12" s="7">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7">
+        <v>4</v>
+      </c>
+      <c r="G12" s="7">
+        <v>5</v>
+      </c>
+      <c r="H12" s="7">
+        <v>4</v>
+      </c>
+      <c r="I12" s="7">
+        <v>4</v>
+      </c>
+      <c r="J12" s="7">
+        <v>7</v>
+      </c>
+      <c r="K12" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="7">
+        <v>12</v>
+      </c>
+      <c r="C13" s="7">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7">
+        <v>8</v>
+      </c>
+      <c r="E13" s="7">
+        <v>13</v>
+      </c>
+      <c r="F13" s="7">
+        <v>10</v>
+      </c>
+      <c r="G13" s="7">
+        <v>8</v>
+      </c>
+      <c r="H13" s="7">
+        <v>9</v>
+      </c>
+      <c r="I13" s="7">
+        <v>15</v>
+      </c>
+      <c r="J13" s="7">
+        <v>11</v>
+      </c>
+      <c r="K13" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="7">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7">
+        <v>13</v>
+      </c>
+      <c r="D14" s="7">
+        <v>8</v>
+      </c>
+      <c r="E14" s="7">
+        <v>13</v>
+      </c>
+      <c r="F14" s="7">
+        <v>10</v>
+      </c>
+      <c r="G14" s="7">
+        <v>8</v>
+      </c>
+      <c r="H14" s="7">
+        <v>9</v>
+      </c>
+      <c r="I14" s="7">
+        <v>15</v>
+      </c>
+      <c r="J14" s="7">
+        <v>11</v>
+      </c>
+      <c r="K14" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="7">
+        <v>56</v>
+      </c>
+      <c r="C16" s="7">
+        <v>44</v>
+      </c>
+      <c r="D16" s="7">
+        <v>41</v>
+      </c>
+      <c r="E16" s="7">
+        <v>35</v>
+      </c>
+      <c r="F16" s="7">
+        <v>33</v>
+      </c>
+      <c r="G16" s="7">
+        <v>43</v>
+      </c>
+      <c r="H16" s="7">
+        <v>24</v>
+      </c>
+      <c r="I16" s="7">
+        <v>39</v>
+      </c>
+      <c r="J16" s="7">
+        <v>28</v>
+      </c>
+      <c r="K16" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="7">
+        <v>25</v>
+      </c>
+      <c r="C17" s="7">
+        <v>21</v>
+      </c>
+      <c r="D17" s="7">
+        <v>15</v>
+      </c>
+      <c r="E17" s="7">
+        <v>7</v>
+      </c>
+      <c r="F17" s="7">
+        <v>10</v>
+      </c>
+      <c r="G17" s="7">
+        <v>13</v>
+      </c>
+      <c r="H17" s="7">
+        <v>11</v>
+      </c>
+      <c r="I17" s="7">
+        <v>21</v>
+      </c>
+      <c r="J17" s="7">
+        <v>11</v>
+      </c>
+      <c r="K17" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="7">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7">
+        <v>5</v>
+      </c>
+      <c r="D18" s="7">
+        <v>6</v>
+      </c>
+      <c r="E18" s="7">
+        <v>3</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="7">
+        <v>2</v>
+      </c>
+      <c r="H18" s="7">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7">
+        <v>4</v>
+      </c>
+      <c r="J18" s="7">
+        <v>4</v>
+      </c>
+      <c r="K18" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="7">
+        <v>5</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="7">
+        <v>3</v>
+      </c>
+      <c r="E19" s="7">
+        <v>8</v>
+      </c>
+      <c r="F19" s="7">
+        <v>5</v>
+      </c>
+      <c r="G19" s="7">
+        <v>6</v>
+      </c>
+      <c r="H19" s="7">
+        <v>4</v>
+      </c>
+      <c r="I19" s="7">
+        <v>5</v>
+      </c>
+      <c r="J19" s="7">
+        <v>1</v>
+      </c>
+      <c r="K19" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="7">
+        <v>4</v>
+      </c>
+      <c r="C20" s="7">
+        <v>2</v>
+      </c>
+      <c r="D20" s="7">
+        <v>2</v>
+      </c>
+      <c r="E20" s="7">
+        <v>4</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2</v>
+      </c>
+      <c r="G20" s="7">
+        <v>9</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7">
+        <v>4</v>
+      </c>
+      <c r="J20" s="7">
+        <v>2</v>
+      </c>
+      <c r="K20" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="7">
+        <v>3</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7">
+        <v>3</v>
+      </c>
+      <c r="G21" s="7">
+        <v>1</v>
+      </c>
+      <c r="H21" s="7">
+        <v>1</v>
+      </c>
+      <c r="I21" s="7">
+        <v>2</v>
+      </c>
+      <c r="J21" s="7">
+        <v>2</v>
+      </c>
+      <c r="K21" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="7">
+        <v>18</v>
+      </c>
+      <c r="C22" s="7">
+        <v>13</v>
+      </c>
+      <c r="D22" s="7">
+        <v>15</v>
+      </c>
+      <c r="E22" s="7">
+        <v>12</v>
+      </c>
+      <c r="F22" s="7">
+        <v>12</v>
+      </c>
+      <c r="G22" s="7">
+        <v>12</v>
+      </c>
+      <c r="H22" s="7">
+        <v>6</v>
+      </c>
+      <c r="I22" s="7">
+        <v>3</v>
+      </c>
+      <c r="J22" s="7">
+        <v>8</v>
+      </c>
+      <c r="K22" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="7">
+        <v>42</v>
+      </c>
+      <c r="C23" s="7">
+        <v>37</v>
+      </c>
+      <c r="D23" s="7">
+        <v>43</v>
+      </c>
+      <c r="E23" s="7">
+        <v>33</v>
+      </c>
+      <c r="F23" s="7">
+        <v>41</v>
+      </c>
+      <c r="G23" s="7">
+        <v>42</v>
+      </c>
+      <c r="H23" s="7">
+        <v>36</v>
+      </c>
+      <c r="I23" s="7">
+        <v>29</v>
+      </c>
+      <c r="J23" s="7">
+        <v>29</v>
+      </c>
+      <c r="K23" s="7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="7">
+        <v>5</v>
+      </c>
+      <c r="C24" s="7">
+        <v>4</v>
+      </c>
+      <c r="D24" s="7">
+        <v>4</v>
+      </c>
+      <c r="E24" s="7">
+        <v>2</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1</v>
+      </c>
+      <c r="G24" s="7">
+        <v>2</v>
+      </c>
+      <c r="H24" s="7">
+        <v>4</v>
+      </c>
+      <c r="I24" s="7">
+        <v>5</v>
+      </c>
+      <c r="J24" s="7">
+        <v>5</v>
+      </c>
+      <c r="K24" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="7">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="7">
+        <v>9</v>
+      </c>
+      <c r="C26" s="7">
+        <v>7</v>
+      </c>
+      <c r="D26" s="7">
+        <v>6</v>
+      </c>
+      <c r="E26" s="7">
+        <v>2</v>
+      </c>
+      <c r="F26" s="7">
+        <v>4</v>
+      </c>
+      <c r="G26" s="7">
+        <v>15</v>
+      </c>
+      <c r="H26" s="7">
+        <v>4</v>
+      </c>
+      <c r="I26" s="7">
+        <v>5</v>
+      </c>
+      <c r="J26" s="7">
+        <v>6</v>
+      </c>
+      <c r="K26" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="7">
+        <v>17</v>
+      </c>
+      <c r="C27" s="7">
+        <v>18</v>
+      </c>
+      <c r="D27" s="7">
+        <v>16</v>
+      </c>
+      <c r="E27" s="7">
+        <v>13</v>
+      </c>
+      <c r="F27" s="7">
+        <v>20</v>
+      </c>
+      <c r="G27" s="7">
+        <v>14</v>
+      </c>
+      <c r="H27" s="7">
+        <v>6</v>
+      </c>
+      <c r="I27" s="7">
+        <v>6</v>
+      </c>
+      <c r="J27" s="7">
+        <v>9</v>
+      </c>
+      <c r="K27" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="7">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>2</v>
+      </c>
+      <c r="D28" s="7">
+        <v>4</v>
+      </c>
+      <c r="E28" s="7">
+        <v>6</v>
+      </c>
+      <c r="F28" s="7">
+        <v>5</v>
+      </c>
+      <c r="G28" s="7">
+        <v>6</v>
+      </c>
+      <c r="H28" s="7">
+        <v>3</v>
+      </c>
+      <c r="I28" s="7">
+        <v>3</v>
+      </c>
+      <c r="J28" s="7">
+        <v>4</v>
+      </c>
+      <c r="K28" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7">
+        <v>5</v>
+      </c>
+      <c r="E29" s="7">
+        <v>2</v>
+      </c>
+      <c r="F29" s="7">
+        <v>3</v>
+      </c>
+      <c r="G29" s="7">
+        <v>2</v>
+      </c>
+      <c r="H29" s="7">
+        <v>4</v>
+      </c>
+      <c r="I29" s="7">
+        <v>4</v>
+      </c>
+      <c r="J29" s="7">
+        <v>1</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="7">
+        <v>7</v>
+      </c>
+      <c r="C30" s="7">
+        <v>5</v>
+      </c>
+      <c r="D30" s="7">
+        <v>8</v>
+      </c>
+      <c r="E30" s="7">
+        <v>8</v>
+      </c>
+      <c r="F30" s="7">
+        <v>8</v>
+      </c>
+      <c r="G30" s="7">
+        <v>3</v>
+      </c>
+      <c r="H30" s="7">
+        <v>15</v>
+      </c>
+      <c r="I30" s="7">
+        <v>6</v>
+      </c>
+      <c r="J30" s="7">
+        <v>4</v>
+      </c>
+      <c r="K30" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="7">
+        <v>36</v>
+      </c>
+      <c r="C31" s="7">
+        <v>44</v>
+      </c>
+      <c r="D31" s="7">
+        <v>41</v>
+      </c>
+      <c r="E31" s="7">
+        <v>45</v>
+      </c>
+      <c r="F31" s="7">
+        <v>30</v>
+      </c>
+      <c r="G31" s="7">
+        <v>31</v>
+      </c>
+      <c r="H31" s="7">
+        <v>23</v>
+      </c>
+      <c r="I31" s="7">
+        <v>32</v>
+      </c>
+      <c r="J31" s="7">
+        <v>20</v>
+      </c>
+      <c r="K31" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="7">
+        <v>7</v>
+      </c>
+      <c r="C32" s="7">
+        <v>14</v>
+      </c>
+      <c r="D32" s="7">
+        <v>19</v>
+      </c>
+      <c r="E32" s="7">
+        <v>13</v>
+      </c>
+      <c r="F32" s="7">
+        <v>8</v>
+      </c>
+      <c r="G32" s="7">
+        <v>6</v>
+      </c>
+      <c r="H32" s="7">
+        <v>7</v>
+      </c>
+      <c r="I32" s="7">
+        <v>5</v>
+      </c>
+      <c r="J32" s="7">
+        <v>2</v>
+      </c>
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="7">
+        <v>7</v>
+      </c>
+      <c r="C33" s="7">
+        <v>12</v>
+      </c>
+      <c r="D33" s="7">
+        <v>16</v>
+      </c>
+      <c r="E33" s="7">
+        <v>11</v>
+      </c>
+      <c r="F33" s="7">
+        <v>7</v>
+      </c>
+      <c r="G33" s="7">
+        <v>2</v>
+      </c>
+      <c r="H33" s="7">
+        <v>3</v>
+      </c>
+      <c r="I33" s="7">
+        <v>5</v>
+      </c>
+      <c r="J33" s="7">
+        <v>2</v>
+      </c>
+      <c r="K33" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1</v>
+      </c>
+      <c r="H34" s="7">
+        <v>1</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="7">
+        <v>2</v>
+      </c>
+      <c r="E35" s="7">
+        <v>2</v>
+      </c>
+      <c r="F35" s="7">
+        <v>1</v>
+      </c>
+      <c r="G35" s="7">
+        <v>3</v>
+      </c>
+      <c r="H35" s="7">
+        <v>2</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="7">
+        <v>2</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H36" s="7">
+        <v>1</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="7">
+        <v>7</v>
+      </c>
+      <c r="C37" s="7">
+        <v>7</v>
+      </c>
+      <c r="D37" s="7">
+        <v>7</v>
+      </c>
+      <c r="E37" s="7">
+        <v>10</v>
+      </c>
+      <c r="F37" s="7">
+        <v>7</v>
+      </c>
+      <c r="G37" s="7">
+        <v>7</v>
+      </c>
+      <c r="H37" s="7">
+        <v>8</v>
+      </c>
+      <c r="I37" s="7">
+        <v>11</v>
+      </c>
+      <c r="J37" s="7">
+        <v>7</v>
+      </c>
+      <c r="K37" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="7">
+        <v>4</v>
+      </c>
+      <c r="C38" s="7">
+        <v>5</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="7">
+        <v>6</v>
+      </c>
+      <c r="F38" s="7">
+        <v>2</v>
+      </c>
+      <c r="G38" s="7">
+        <v>2</v>
+      </c>
+      <c r="H38" s="7">
+        <v>2</v>
+      </c>
+      <c r="I38" s="7">
+        <v>9</v>
+      </c>
+      <c r="J38" s="7">
+        <v>2</v>
+      </c>
+      <c r="K38" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="7">
+        <v>3</v>
+      </c>
+      <c r="C39" s="7">
+        <v>2</v>
+      </c>
+      <c r="D39" s="7">
+        <v>5</v>
+      </c>
+      <c r="E39" s="7">
+        <v>4</v>
+      </c>
+      <c r="F39" s="7">
+        <v>5</v>
+      </c>
+      <c r="G39" s="7">
+        <v>5</v>
+      </c>
+      <c r="H39" s="7">
+        <v>6</v>
+      </c>
+      <c r="I39" s="7">
+        <v>2</v>
+      </c>
+      <c r="J39" s="7">
+        <v>5</v>
+      </c>
+      <c r="K39" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="7">
+        <v>2</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" s="7">
+        <v>22</v>
+      </c>
+      <c r="C41" s="7">
+        <v>23</v>
+      </c>
+      <c r="D41" s="7">
+        <v>15</v>
+      </c>
+      <c r="E41" s="7">
+        <v>22</v>
+      </c>
+      <c r="F41" s="7">
+        <v>15</v>
+      </c>
+      <c r="G41" s="7">
+        <v>18</v>
+      </c>
+      <c r="H41" s="7">
+        <v>8</v>
+      </c>
+      <c r="I41" s="7">
+        <v>16</v>
+      </c>
+      <c r="J41" s="7">
+        <v>11</v>
+      </c>
+      <c r="K41" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="7">
+        <v>11</v>
+      </c>
+      <c r="C42" s="7">
+        <v>13</v>
+      </c>
+      <c r="D42" s="7">
+        <v>10</v>
+      </c>
+      <c r="E42" s="7">
+        <v>12</v>
+      </c>
+      <c r="F42" s="7">
+        <v>5</v>
+      </c>
+      <c r="G42" s="7">
+        <v>13</v>
+      </c>
+      <c r="H42" s="7">
+        <v>4</v>
+      </c>
+      <c r="I42" s="7">
+        <v>9</v>
+      </c>
+      <c r="J42" s="7">
+        <v>9</v>
+      </c>
+      <c r="K42" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="9">
+        <v>11</v>
+      </c>
+      <c r="C43" s="9">
+        <v>10</v>
+      </c>
+      <c r="D43" s="9">
+        <v>5</v>
+      </c>
+      <c r="E43" s="9">
+        <v>10</v>
+      </c>
+      <c r="F43" s="9">
+        <v>10</v>
+      </c>
+      <c r="G43" s="9">
+        <v>5</v>
+      </c>
+      <c r="H43" s="9">
+        <v>4</v>
+      </c>
+      <c r="I43" s="9">
+        <v>7</v>
+      </c>
+      <c r="J43" s="9">
+        <v>2</v>
+      </c>
+      <c r="K43" s="9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B0A253-F524-2742-9601-4FA210832464}">
   <dimension ref="A1:AB42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2096,12 +3953,1507 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F687377F-5944-0D42-B9FF-1F606B108A1C}">
+  <dimension ref="A1:AB42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection sqref="A1:K42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E1" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F1" s="2">
+        <v>2018</v>
+      </c>
+      <c r="G1" s="2">
+        <v>2017</v>
+      </c>
+      <c r="H1" s="2">
+        <v>2016</v>
+      </c>
+      <c r="I1" s="2">
+        <v>2015</v>
+      </c>
+      <c r="J1" s="2">
+        <v>2014</v>
+      </c>
+      <c r="K1" s="2">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2">
+        <v>611</v>
+      </c>
+      <c r="C2">
+        <v>579</v>
+      </c>
+      <c r="D2">
+        <v>501</v>
+      </c>
+      <c r="E2">
+        <v>472</v>
+      </c>
+      <c r="F2">
+        <v>428</v>
+      </c>
+      <c r="G2">
+        <v>410</v>
+      </c>
+      <c r="H2">
+        <v>595</v>
+      </c>
+      <c r="I2">
+        <v>725</v>
+      </c>
+      <c r="J2">
+        <v>563</v>
+      </c>
+      <c r="K2">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3">
+        <v>324</v>
+      </c>
+      <c r="C3">
+        <v>301</v>
+      </c>
+      <c r="D3">
+        <v>274</v>
+      </c>
+      <c r="E3">
+        <v>280</v>
+      </c>
+      <c r="F3">
+        <v>252</v>
+      </c>
+      <c r="G3">
+        <v>252</v>
+      </c>
+      <c r="H3">
+        <v>335</v>
+      </c>
+      <c r="I3">
+        <v>370</v>
+      </c>
+      <c r="J3">
+        <v>277</v>
+      </c>
+      <c r="K3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4">
+        <v>287</v>
+      </c>
+      <c r="C4">
+        <v>278</v>
+      </c>
+      <c r="D4">
+        <v>227</v>
+      </c>
+      <c r="E4">
+        <v>192</v>
+      </c>
+      <c r="F4">
+        <v>176</v>
+      </c>
+      <c r="G4">
+        <v>158</v>
+      </c>
+      <c r="H4">
+        <v>260</v>
+      </c>
+      <c r="I4">
+        <v>355</v>
+      </c>
+      <c r="J4">
+        <v>286</v>
+      </c>
+      <c r="K4">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5">
+        <v>553</v>
+      </c>
+      <c r="C5">
+        <v>536</v>
+      </c>
+      <c r="D5">
+        <v>434</v>
+      </c>
+      <c r="E5">
+        <v>422</v>
+      </c>
+      <c r="F5">
+        <v>387</v>
+      </c>
+      <c r="G5">
+        <v>369</v>
+      </c>
+      <c r="H5">
+        <v>522</v>
+      </c>
+      <c r="I5">
+        <v>655</v>
+      </c>
+      <c r="J5">
+        <v>496</v>
+      </c>
+      <c r="K5">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6">
+        <v>343</v>
+      </c>
+      <c r="C6">
+        <v>322</v>
+      </c>
+      <c r="D6">
+        <v>280</v>
+      </c>
+      <c r="E6">
+        <v>279</v>
+      </c>
+      <c r="F6">
+        <v>252</v>
+      </c>
+      <c r="G6">
+        <v>235</v>
+      </c>
+      <c r="H6">
+        <v>347</v>
+      </c>
+      <c r="I6">
+        <v>389</v>
+      </c>
+      <c r="J6">
+        <v>261</v>
+      </c>
+      <c r="K6">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7">
+        <v>208</v>
+      </c>
+      <c r="C7">
+        <v>210</v>
+      </c>
+      <c r="D7">
+        <v>149</v>
+      </c>
+      <c r="E7">
+        <v>138</v>
+      </c>
+      <c r="F7">
+        <v>128</v>
+      </c>
+      <c r="G7">
+        <v>129</v>
+      </c>
+      <c r="H7">
+        <v>171</v>
+      </c>
+      <c r="I7">
+        <v>260</v>
+      </c>
+      <c r="J7">
+        <v>229</v>
+      </c>
+      <c r="K7">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>26</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>24</v>
+      </c>
+      <c r="I9">
+        <v>27</v>
+      </c>
+      <c r="J9">
+        <v>39</v>
+      </c>
+      <c r="K9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10">
+        <v>83</v>
+      </c>
+      <c r="C10">
+        <v>83</v>
+      </c>
+      <c r="D10">
+        <v>64</v>
+      </c>
+      <c r="E10">
+        <v>49</v>
+      </c>
+      <c r="F10">
+        <v>56</v>
+      </c>
+      <c r="G10">
+        <v>54</v>
+      </c>
+      <c r="H10">
+        <v>67</v>
+      </c>
+      <c r="I10">
+        <v>90</v>
+      </c>
+      <c r="J10">
+        <v>63</v>
+      </c>
+      <c r="K10">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12">
+        <v>74</v>
+      </c>
+      <c r="C12">
+        <v>76</v>
+      </c>
+      <c r="D12">
+        <v>51</v>
+      </c>
+      <c r="E12">
+        <v>53</v>
+      </c>
+      <c r="F12">
+        <v>45</v>
+      </c>
+      <c r="G12">
+        <v>54</v>
+      </c>
+      <c r="H12">
+        <v>77</v>
+      </c>
+      <c r="I12">
+        <v>118</v>
+      </c>
+      <c r="J12">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>8</v>
+      </c>
+      <c r="K13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+      <c r="K14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15">
+        <v>58</v>
+      </c>
+      <c r="C15">
+        <v>43</v>
+      </c>
+      <c r="D15">
+        <v>67</v>
+      </c>
+      <c r="E15">
+        <v>50</v>
+      </c>
+      <c r="F15">
+        <v>41</v>
+      </c>
+      <c r="G15">
+        <v>41</v>
+      </c>
+      <c r="H15">
+        <v>73</v>
+      </c>
+      <c r="I15">
+        <v>70</v>
+      </c>
+      <c r="J15">
+        <v>67</v>
+      </c>
+      <c r="K15">
+        <v>56</v>
+      </c>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16">
+        <v>473</v>
+      </c>
+      <c r="C16">
+        <v>456</v>
+      </c>
+      <c r="D16">
+        <v>415</v>
+      </c>
+      <c r="E16">
+        <v>402</v>
+      </c>
+      <c r="F16">
+        <v>368</v>
+      </c>
+      <c r="G16">
+        <v>352</v>
+      </c>
+      <c r="H16">
+        <v>543</v>
+      </c>
+      <c r="I16">
+        <v>644</v>
+      </c>
+      <c r="J16">
+        <v>469</v>
+      </c>
+      <c r="K16">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17">
+        <v>354</v>
+      </c>
+      <c r="C17">
+        <v>343</v>
+      </c>
+      <c r="D17">
+        <v>302</v>
+      </c>
+      <c r="E17">
+        <v>285</v>
+      </c>
+      <c r="F17">
+        <v>278</v>
+      </c>
+      <c r="G17">
+        <v>280</v>
+      </c>
+      <c r="H17">
+        <v>427</v>
+      </c>
+      <c r="I17">
+        <v>516</v>
+      </c>
+      <c r="J17">
+        <v>340</v>
+      </c>
+      <c r="K17">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>58</v>
+      </c>
+      <c r="J19">
+        <v>62</v>
+      </c>
+      <c r="K19">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>51</v>
+      </c>
+      <c r="I20">
+        <v>51</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21">
+        <v>187</v>
+      </c>
+      <c r="C21">
+        <v>179</v>
+      </c>
+      <c r="D21">
+        <v>157</v>
+      </c>
+      <c r="E21">
+        <v>150</v>
+      </c>
+      <c r="F21">
+        <v>147</v>
+      </c>
+      <c r="G21">
+        <v>152</v>
+      </c>
+      <c r="H21">
+        <v>121</v>
+      </c>
+      <c r="I21">
+        <v>89</v>
+      </c>
+      <c r="J21">
+        <v>52</v>
+      </c>
+      <c r="K21">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23">
+        <v>9</v>
+      </c>
+      <c r="I23">
+        <v>15</v>
+      </c>
+      <c r="J23">
+        <v>15</v>
+      </c>
+      <c r="K23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>8</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27">
+        <v>39</v>
+      </c>
+      <c r="C27">
+        <v>19</v>
+      </c>
+      <c r="D27">
+        <v>18</v>
+      </c>
+      <c r="E27">
+        <v>18</v>
+      </c>
+      <c r="F27">
+        <v>16</v>
+      </c>
+      <c r="G27">
+        <v>16</v>
+      </c>
+      <c r="H27">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>14</v>
+      </c>
+      <c r="J27">
+        <v>17</v>
+      </c>
+      <c r="K27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>6</v>
+      </c>
+      <c r="I28">
+        <v>12</v>
+      </c>
+      <c r="J28">
+        <v>15</v>
+      </c>
+      <c r="K28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29">
+        <v>68</v>
+      </c>
+      <c r="C29">
+        <v>90</v>
+      </c>
+      <c r="D29">
+        <v>76</v>
+      </c>
+      <c r="E29">
+        <v>76</v>
+      </c>
+      <c r="F29">
+        <v>83</v>
+      </c>
+      <c r="G29">
+        <v>92</v>
+      </c>
+      <c r="H29">
+        <v>220</v>
+      </c>
+      <c r="I29">
+        <v>271</v>
+      </c>
+      <c r="J29">
+        <v>174</v>
+      </c>
+      <c r="K29">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30">
+        <v>119</v>
+      </c>
+      <c r="C30">
+        <v>113</v>
+      </c>
+      <c r="D30">
+        <v>113</v>
+      </c>
+      <c r="E30">
+        <v>117</v>
+      </c>
+      <c r="F30">
+        <v>90</v>
+      </c>
+      <c r="G30">
+        <v>72</v>
+      </c>
+      <c r="H30">
+        <v>116</v>
+      </c>
+      <c r="I30">
+        <v>128</v>
+      </c>
+      <c r="J30">
+        <v>129</v>
+      </c>
+      <c r="K30">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>6</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="G32">
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="I32">
+        <v>11</v>
+      </c>
+      <c r="J32">
+        <v>13</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>28</v>
+      </c>
+      <c r="D34">
+        <v>28</v>
+      </c>
+      <c r="E34">
+        <v>32</v>
+      </c>
+      <c r="F34">
+        <v>22</v>
+      </c>
+      <c r="G34">
+        <v>23</v>
+      </c>
+      <c r="H34">
+        <v>29</v>
+      </c>
+      <c r="I34">
+        <v>37</v>
+      </c>
+      <c r="J34">
+        <v>46</v>
+      </c>
+      <c r="K34">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35">
+        <v>49</v>
+      </c>
+      <c r="C35">
+        <v>42</v>
+      </c>
+      <c r="D35">
+        <v>48</v>
+      </c>
+      <c r="E35">
+        <v>60</v>
+      </c>
+      <c r="F35">
+        <v>41</v>
+      </c>
+      <c r="G35">
+        <v>27</v>
+      </c>
+      <c r="H35">
+        <v>60</v>
+      </c>
+      <c r="I35">
+        <v>51</v>
+      </c>
+      <c r="J35">
+        <v>52</v>
+      </c>
+      <c r="K35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>16</v>
+      </c>
+      <c r="D36">
+        <v>13</v>
+      </c>
+      <c r="E36">
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <v>10</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37">
+        <v>16</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>13</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <v>7</v>
+      </c>
+      <c r="G37">
+        <v>12</v>
+      </c>
+      <c r="H37">
+        <v>16</v>
+      </c>
+      <c r="I37">
+        <v>20</v>
+      </c>
+      <c r="J37">
+        <v>15</v>
+      </c>
+      <c r="K37">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>9</v>
+      </c>
+      <c r="J38">
+        <v>3</v>
+      </c>
+      <c r="K38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40">
+        <v>138</v>
+      </c>
+      <c r="C40">
+        <v>123</v>
+      </c>
+      <c r="D40">
+        <v>86</v>
+      </c>
+      <c r="E40">
+        <v>70</v>
+      </c>
+      <c r="F40">
+        <v>60</v>
+      </c>
+      <c r="G40">
+        <v>58</v>
+      </c>
+      <c r="H40">
+        <v>52</v>
+      </c>
+      <c r="I40">
+        <v>81</v>
+      </c>
+      <c r="J40">
+        <v>94</v>
+      </c>
+      <c r="K40">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41">
+        <v>128</v>
+      </c>
+      <c r="C41">
+        <v>111</v>
+      </c>
+      <c r="D41">
+        <v>77</v>
+      </c>
+      <c r="E41">
+        <v>58</v>
+      </c>
+      <c r="F41">
+        <v>49</v>
+      </c>
+      <c r="G41">
+        <v>49</v>
+      </c>
+      <c r="H41">
+        <v>39</v>
+      </c>
+      <c r="I41">
+        <v>62</v>
+      </c>
+      <c r="J41">
+        <v>79</v>
+      </c>
+      <c r="K41">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>12</v>
+      </c>
+      <c r="D42">
+        <v>9</v>
+      </c>
+      <c r="E42">
+        <v>12</v>
+      </c>
+      <c r="F42">
+        <v>11</v>
+      </c>
+      <c r="G42">
+        <v>9</v>
+      </c>
+      <c r="H42">
+        <v>13</v>
+      </c>
+      <c r="I42">
+        <v>19</v>
+      </c>
+      <c r="J42">
+        <v>15</v>
+      </c>
+      <c r="K42">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78A1C2C-BD8B-6348-BC78-C4C37A4E847A}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2177,7 +5529,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B3">
@@ -2317,7 +5669,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B7">
@@ -2457,7 +5809,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B11">
@@ -2597,7 +5949,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B15">
@@ -2737,7 +6089,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B19">
@@ -2777,12 +6129,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F607ED8E-C479-4541-87B6-0A1C52968ED2}">
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>